<commit_message>
Fixato errore in SimpleGridObject
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/readloocup_template.xlsx
+++ b/src/main/resources/excel/readloocup_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Workspace\ExcelFromXMLObject\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F767FE71-4D42-42E2-BB04-32D1A7D6A0EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AF4F13-0D40-4BF9-8D5C-44F709F93BA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="3825" windowWidth="21600" windowHeight="11385" xr2:uid="{D048C21C-6F62-426E-A658-66B2421AE3F1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D048C21C-6F62-426E-A658-66B2421AE3F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,8 +74,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="grid.getTable()" var="table" lastCell="A5")
-jx:each(items="table" var="String" lastCell="A5" direction="RIGHT")</t>
+jx:each(items="grid.getTable()" var="table" lastCell="A5" direction="RIGHT")
+jx:each(items="table" var="String" lastCell="A5" direction="DOWN")</t>
         </r>
       </text>
     </comment>
@@ -494,7 +494,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>